<commit_message>
Finish Email with Attachment
</commit_message>
<xml_diff>
--- a/public/exportBackupRequestIdsRecord.xlsx
+++ b/public/exportBackupRequestIdsRecord.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -689,9 +689,501 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>6260261fcb5c2af8bf638441</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Song Wendy</v>
+      </c>
+      <c r="C8" t="str">
+        <v>North Korea</v>
+      </c>
+      <c r="D8" t="str">
+        <v>songwendy@g.c</v>
+      </c>
+      <c r="E8">
+        <v>435</v>
+      </c>
+      <c r="F8">
+        <v>98</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Single</v>
+      </c>
+      <c r="H8" t="str">
+        <v>No Reason</v>
+      </c>
+      <c r="I8" t="str">
+        <v>3434</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K8" t="str">
+        <v>image_1650468383148_gcash-merged.pdf</v>
+      </c>
+      <c r="L8" t="str">
+        <v>April 20th 2022</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>6260b3d7979a8f72c0e5f8ee</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Bae Irene</v>
+      </c>
+      <c r="C9" t="str">
+        <v>South Korea</v>
+      </c>
+      <c r="D9" t="str">
+        <v>baeirene@g.c</v>
+      </c>
+      <c r="E9">
+        <v>43090</v>
+      </c>
+      <c r="F9">
+        <v>29</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Single</v>
+      </c>
+      <c r="H9" t="str">
+        <v>No Reason</v>
+      </c>
+      <c r="I9" t="str">
+        <v>25366523fdfdf</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K9" t="str">
+        <v>image_1650504663047_gcash-merged.pdf</v>
+      </c>
+      <c r="L9" t="str">
+        <v>April 21st 2022</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>6260b48dcdeded58dd9be7c4</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Juliet Mediona Nicanor</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Rosario Village, Botong Francisco Ave</v>
+      </c>
+      <c r="D10" t="str">
+        <v>julietnicanor1996@gmail.com</v>
+      </c>
+      <c r="E10">
+        <v>639395029337</v>
+      </c>
+      <c r="F10">
+        <v>23</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Single</v>
+      </c>
+      <c r="H10" t="str">
+        <v>No Reason</v>
+      </c>
+      <c r="I10" t="str">
+        <v>dsds</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K10" t="str">
+        <v>image_1650504845890_gcash-merged.pdf</v>
+      </c>
+      <c r="L10" t="str">
+        <v>April 21st 2022</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>6260b9387982862243e193d9</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Juliet Mediona Nicanor</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Rosario Village, Botong Francisco Ave</v>
+      </c>
+      <c r="D11" t="str">
+        <v>julietnicanor1996@gmail.com</v>
+      </c>
+      <c r="E11">
+        <v>639395029337</v>
+      </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Single</v>
+      </c>
+      <c r="H11" t="str">
+        <v>dsds</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Hellow</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K11" t="str">
+        <v>image_1650506040165_gcash-merged.pdf</v>
+      </c>
+      <c r="L11" t="str">
+        <v>April 21st 2022</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>6260ba75443489731d5dd848</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Juliet Mediona Nicanor</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Rosario Village, Botong Francisco Ave</v>
+      </c>
+      <c r="D12" t="str">
+        <v>julietnicanor1996@gmail.com</v>
+      </c>
+      <c r="E12">
+        <v>639395029337</v>
+      </c>
+      <c r="F12">
+        <v>23</v>
+      </c>
+      <c r="G12" t="str">
+        <v>dsd</v>
+      </c>
+      <c r="H12" t="str">
+        <v>No Reason</v>
+      </c>
+      <c r="I12" t="str">
+        <v>sas</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K12" t="str">
+        <v>image_1650506357140_gcash-merged.pdf</v>
+      </c>
+      <c r="L12" t="str">
+        <v>April 21st 2022</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>62613a069b232834da3435b1</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Juliet Mediona Nicanor</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Rosario Village, Botong Francisco Ave</v>
+      </c>
+      <c r="D13" t="str">
+        <v>julietnicanor1996@gmail.com</v>
+      </c>
+      <c r="E13">
+        <v>639395029337</v>
+      </c>
+      <c r="F13">
+        <v>23</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Single</v>
+      </c>
+      <c r="H13" t="str">
+        <v>dsds</v>
+      </c>
+      <c r="I13" t="str">
+        <v>sasa</v>
+      </c>
+      <c r="J13" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K13" t="str">
+        <v>image_1650539014655_gcash-merged.pdf</v>
+      </c>
+      <c r="L13" t="str">
+        <v>April 21st 2022</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>62613a6fc4a527c4d9811a56</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Juliet Mediona Nicanor</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Rosario Village, Botong Francisco Ave</v>
+      </c>
+      <c r="D14" t="str">
+        <v>julietnicanor1996@gmail.com</v>
+      </c>
+      <c r="E14">
+        <v>639395029337</v>
+      </c>
+      <c r="F14">
+        <v>23</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Single</v>
+      </c>
+      <c r="H14" t="str">
+        <v>No Reason</v>
+      </c>
+      <c r="I14" t="str">
+        <v>dsds</v>
+      </c>
+      <c r="J14" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K14" t="str">
+        <v>image_1650539119186_gcash-merged.pdf</v>
+      </c>
+      <c r="L14" t="str">
+        <v>April 21st 2022</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>62613bc3d1a757dc31a3791c</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Juliet Mediona Nicanor</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Rosario Village, Botong Francisco Ave</v>
+      </c>
+      <c r="D15" t="str">
+        <v>julietnicanor1996@gmail.com</v>
+      </c>
+      <c r="E15">
+        <v>639395029337</v>
+      </c>
+      <c r="F15">
+        <v>23</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Single</v>
+      </c>
+      <c r="H15" t="str">
+        <v>No Reason</v>
+      </c>
+      <c r="I15" t="str">
+        <v>fdfd</v>
+      </c>
+      <c r="J15" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K15" t="str">
+        <v>image_1650539459882_gcash-merged.pdf</v>
+      </c>
+      <c r="L15" t="str">
+        <v>April 21st 2022</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>62613cad6ad815c490fa8b18</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Juliet Mediona Nicanor</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Rosario Village, Botong Francisco Ave</v>
+      </c>
+      <c r="D16" t="str">
+        <v>julietnicanor1996@gmail.com</v>
+      </c>
+      <c r="E16">
+        <v>639395029337</v>
+      </c>
+      <c r="F16">
+        <v>23</v>
+      </c>
+      <c r="G16" t="str">
+        <v>dsd</v>
+      </c>
+      <c r="H16" t="str">
+        <v>No Reason</v>
+      </c>
+      <c r="I16" t="str">
+        <v>Hellow</v>
+      </c>
+      <c r="J16" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K16" t="str">
+        <v>image_1650539693584_gcash-merged.pdf</v>
+      </c>
+      <c r="L16" t="str">
+        <v>April 21st 2022</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>626227a8f9a6dab50754a5a5</v>
+      </c>
+      <c r="B17" t="str">
+        <v xml:space="preserve">  Duterte, Rodrigo    </v>
+      </c>
+      <c r="C17" t="str">
+        <v>Davao</v>
+      </c>
+      <c r="D17" t="str">
+        <v>duterts@g.c</v>
+      </c>
+      <c r="E17">
+        <v>49249</v>
+      </c>
+      <c r="F17">
+        <v>79</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Married</v>
+      </c>
+      <c r="H17" t="str">
+        <v>No Reason</v>
+      </c>
+      <c r="I17" t="str">
+        <v>94749324</v>
+      </c>
+      <c r="J17" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K17" t="str">
+        <v>image_1650599848104_gcash-merged.pdf</v>
+      </c>
+      <c r="L17" t="str">
+        <v>April 22nd 2022</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>626233aac2b270ef48934036</v>
+      </c>
+      <c r="B18" t="str">
+        <v xml:space="preserve"> Manoban, Chittip  </v>
+      </c>
+      <c r="C18" t="str">
+        <v>Thailand</v>
+      </c>
+      <c r="D18" t="str">
+        <v>chits@g.c</v>
+      </c>
+      <c r="E18">
+        <v>48926489349837</v>
+      </c>
+      <c r="F18">
+        <v>78</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Married</v>
+      </c>
+      <c r="H18" t="str">
+        <v>No Reason</v>
+      </c>
+      <c r="I18" t="str">
+        <v>r454854d</v>
+      </c>
+      <c r="J18" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K18" t="str">
+        <v>image_1650602922301_gcash-merged.pdf</v>
+      </c>
+      <c r="L18" t="str">
+        <v>April 22nd 2022</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>626238453e5f50cf8f9a50cd</v>
+      </c>
+      <c r="B19" t="str">
+        <v xml:space="preserve"> thelma m. nicanor  </v>
+      </c>
+      <c r="C19" t="str">
+        <v>Rosario Village</v>
+      </c>
+      <c r="D19" t="str">
+        <v>thelmanicanor@gmail.com</v>
+      </c>
+      <c r="E19">
+        <v>65656768769789</v>
+      </c>
+      <c r="F19">
+        <v>59</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Married</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Identification</v>
+      </c>
+      <c r="I19" t="str">
+        <v>567678678754545</v>
+      </c>
+      <c r="J19" t="str">
+        <v>Pending</v>
+      </c>
+      <c r="K19" t="str">
+        <v>image_1650604101967_gcash-merged.pdf</v>
+      </c>
+      <c r="L19" t="str">
+        <v>April 22nd 2022</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>